<commit_message>
Updated Tracking Sheet with Vidushi's Task Details
</commit_message>
<xml_diff>
--- a/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
+++ b/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aakash/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal DAta\Downloads\study\SJSU\SEM 1\CMPE 243\cmpe243_techsavy_rc_car\Tracking_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F48ED5-60CA-FA45-84BE-EE0BA6260DFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{8319778D-1403-F846-B2D2-4A73FA8E7C62}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Defines" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tracking Sheet'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -94,9 +93,6 @@
     <t>Halak</t>
   </si>
   <si>
-    <t>Vidhushi</t>
-  </si>
-  <si>
     <t>Jay</t>
   </si>
   <si>
@@ -116,9 +112,6 @@
   </si>
   <si>
     <t>SENSOR</t>
-  </si>
-  <si>
-    <t>GPS</t>
   </si>
   <si>
     <t>BRIDGE</t>
@@ -138,16 +131,54 @@
   <si>
     <t>1. Interfacing Ultrasound HC-SR04 sensor with Sjone board.
 2. Interfacing MaxBotix sensor with Sjone board.</t>
+  </si>
+  <si>
+    <t>Vidushi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidushi </t>
+  </si>
+  <si>
+    <t>Almost Full Day</t>
+  </si>
+  <si>
+    <t>1. Interfacing of Bluetooth HC-05 Module withUBS TTL Convertor to configure Module.
+2. Worked on Command Mode of HC-05 and configured with name Tech_Savy and changed config setting to 38400.
+3. Refactoring of code for Bridge communication
+4. Implemented C wrapper for UART2.cpp, uart_dev.cpp and for switch and LED files. 
+5. Testing done with Sample HC-05 BLE Android Application.</t>
+  </si>
+  <si>
+    <t>GPS/Compass/Bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Updated wiki schedule and BOM
+2. Updated High Level Software Architecture and Team Member details on Wiki. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Interfacing of Bluetooth HC-05 Module with Sjone board and 5V power supply.
+2. Worked on Data Mode(Rx/Tx) of HC-05.
+3. Tested interfacing and working(Rx/TX) with Serial Monitor.
+</t>
+  </si>
+  <si>
+    <t>WIKI Report</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Interfacing, Coding &amp; Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +189,21 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -220,17 +266,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,21 +594,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CF6FA8-359C-CA44-B2B1-E3F3F8AD768C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.69921875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -570,9 +619,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -581,9 +630,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -592,80 +641,80 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -676,26 +725,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE97011-BA77-D547-BA88-CF948621BC01}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -708,7 +757,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -718,77 +767,141 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
         <v>43553</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="8">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="8">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>43553</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="8">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+    <row r="4" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>43553</v>
       </c>
-      <c r="B3" s="3">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="3">
+      <c r="E4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="8">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>43554</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="6" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>43555</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{3033DFEC-9D26-1C4D-B215-0C7263F75299}"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!" xr:uid="{119EB927-DEC7-3044-B21F-ECD44825B96D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!">
           <x14:formula1>
             <xm:f>Defines!$C$2:$C$12</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D44B1E4-A866-EF42-80B4-E16435628A9C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Defines!$B$2:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{293BC0E0-5679-E54B-A23C-B761449467B3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Defines!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!" xr:uid="{3094A77C-4C1B-6348-84C1-AEE5F266C21C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!">
           <x14:formula1>
             <xm:f>Defines!$C$2:$C50</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updated tracking sheet & Bridge Communication With Wrapper
</commit_message>
<xml_diff>
--- a/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
+++ b/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aakash/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal DAta\Downloads\study\SJSU\SEM 1\CMPE 243\cmpe243_techsavy_rc_car\Tracking_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F48ED5-60CA-FA45-84BE-EE0BA6260DFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{8319778D-1403-F846-B2D2-4A73FA8E7C62}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Defines" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tracking Sheet'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -94,9 +93,6 @@
     <t>Halak</t>
   </si>
   <si>
-    <t>Vidhushi</t>
-  </si>
-  <si>
     <t>Jay</t>
   </si>
   <si>
@@ -116,9 +112,6 @@
   </si>
   <si>
     <t>SENSOR</t>
-  </si>
-  <si>
-    <t>GPS</t>
   </si>
   <si>
     <t>BRIDGE</t>
@@ -138,16 +131,54 @@
   <si>
     <t>1. Interfacing Ultrasound HC-SR04 sensor with Sjone board.
 2. Interfacing MaxBotix sensor with Sjone board.</t>
+  </si>
+  <si>
+    <t>Vidushi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidushi </t>
+  </si>
+  <si>
+    <t>Almost Full Day</t>
+  </si>
+  <si>
+    <t>1. Interfacing of Bluetooth HC-05 Module withUBS TTL Convertor to configure Module.
+2. Worked on Command Mode of HC-05 and configured with name Tech_Savy and changed config setting to 38400.
+3. Refactoring of code for Bridge communication
+4. Implemented C wrapper for UART2.cpp, uart_dev.cpp and for switch and LED files. 
+5. Testing done with Sample HC-05 BLE Android Application.</t>
+  </si>
+  <si>
+    <t>GPS/Compass/Bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Updated wiki schedule and BOM
+2. Updated High Level Software Architecture and Team Member details on Wiki. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Interfacing of Bluetooth HC-05 Module with Sjone board and 5V power supply.
+2. Worked on Data Mode(Rx/Tx) of HC-05.
+3. Tested interfacing and working(Rx/TX) with Serial Monitor.
+</t>
+  </si>
+  <si>
+    <t>WIKI Report</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Interfacing, Coding &amp; Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +189,21 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -220,17 +266,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,21 +594,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CF6FA8-359C-CA44-B2B1-E3F3F8AD768C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.69921875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -570,9 +619,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -581,9 +630,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -592,80 +641,80 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -676,26 +725,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE97011-BA77-D547-BA88-CF948621BC01}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -708,7 +757,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -718,77 +767,141 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
         <v>43553</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="8">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="8">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>43553</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="8">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+    <row r="4" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>43553</v>
       </c>
-      <c r="B3" s="3">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="3">
+      <c r="E4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="8">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>43554</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="8">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="6" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>43555</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{3033DFEC-9D26-1C4D-B215-0C7263F75299}"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!" xr:uid="{119EB927-DEC7-3044-B21F-ECD44825B96D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!">
           <x14:formula1>
             <xm:f>Defines!$C$2:$C$12</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D44B1E4-A866-EF42-80B4-E16435628A9C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Defines!$B$2:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{293BC0E0-5679-E54B-A23C-B761449467B3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Defines!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!" xr:uid="{3094A77C-4C1B-6348-84C1-AEE5F266C21C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!">
           <x14:formula1>
             <xm:f>Defines!$C$2:$C50</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Vidushi Updated Time Sheet
</commit_message>
<xml_diff>
--- a/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
+++ b/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_Project\CMPE-243\cmpe243_techsavy_rc_car\Tracking_sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvdn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B97D116-4784-4603-8E93-771AF4E00037}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Defines" sheetId="2" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -180,13 +179,62 @@
 3. Displayed the discovered bluetooth devices in a list view</t>
   </si>
   <si>
-    <t>Bridge</t>
+    <t>1. Pushed Bridge code to gitlab
+2. Hardware Interfaced compass with Sjone Board (5v)</t>
+  </si>
+  <si>
+    <t>Documentation &amp; Interfacing</t>
+  </si>
+  <si>
+    <t>BRIDGE &amp; 
+GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go through CMPS 11 datasheet in i2c &amp; Serial Mode and read about it register settings and configurations </t>
+  </si>
+  <si>
+    <t>CMPS 11 - GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Sheet Reviewing </t>
+  </si>
+  <si>
+    <t>1. Updated wiki report with Project Title details and Car Top &amp; side views.
+2. Added Abstract and How self driving car works on Wiki.
+3. Added Introduction &amp; onjectives of Tech Savy on Wiki with High Level System Design.</t>
+  </si>
+  <si>
+    <t>1. Updated wiki report with  Team Members &amp; Technical Responsibilities.
+2. Updated wiki report with  Team Members &amp;   Administrative Responsibilities.
+3. Updated wiki report with  Team Deliverables Schedule.
+4. Added BILL OF MATERIALS (GENERAL PARTS) and Details on the Wiki.
+5. Changed the Wiki Font , format and design for our team and added color codes for all modules.</t>
+  </si>
+  <si>
+    <t>GEO - CMPS11</t>
+  </si>
+  <si>
+    <t>1. Interfacing of CMPS11 with SJONE board on 3.3V.
+2. Interfaced &amp; Implement I2C Mode with CMP11 on SJOne. 
+3. Worked on all axis Calibration of CMPS11 using registers 0xF0, 0xF5 and 0xF6.
+4. Implemented start &amp; stop caliberation mode for CMPS 11 using command registers on SWITCH.
+5. Implemented factory caliberation mode for CMPS11 on Switch in order to revert caliberation.</t>
+  </si>
+  <si>
+    <t>1. Study &amp; Implemented I2C Read/Write functions for CMPS11.
+2. Implemented Heading Angle Calculation Functionality for CMPS11.
+3. Refactoring of code for Geo Controller.
+4. Implemented C wrapper for I2C2.cpp.</t>
+  </si>
+  <si>
+    <t>1. Updated wiki report with  Team Deliverables Schedule Till Final Demo
+2. Updated HW Block Diagrams for Bluetooth and Geo Controller</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
@@ -263,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,7 +341,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -738,12 +785,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -830,7 +877,9 @@
       <c r="A4" s="7">
         <v>43553</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="8">
+        <v>5</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>42</v>
       </c>
@@ -851,7 +900,9 @@
       <c r="A5" s="7">
         <v>43554</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8">
+        <v>5</v>
+      </c>
       <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
@@ -872,7 +923,9 @@
       <c r="A6" s="7">
         <v>43555</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
       <c r="C6" s="8" t="s">
         <v>43</v>
       </c>
@@ -889,52 +942,216 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+    <row r="7" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>43555</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="E7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>43556</v>
+      </c>
+      <c r="B8" s="8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>43557</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>43558</v>
+      </c>
+      <c r="B10" s="8">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>43559</v>
+      </c>
+      <c r="B11" s="8">
+        <v>5</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="8">
+        <v>4</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>43560</v>
+      </c>
+      <c r="B12" s="8">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="8">
+        <v>4</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>43561</v>
+      </c>
+      <c r="B13" s="8">
+        <v>5</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="8">
+        <v>4</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>43563</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="8">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!">
           <x14:formula1>
             <xm:f>Defines!$C$2:$C$12</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Defines!$B$2:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Defines!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activity" prompt="Please see the dropdown!">
           <x14:formula1>
             <xm:f>Defines!$C$2:$C50</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Added Vatsal's timesheet in tracking
</commit_message>
<xml_diff>
--- a/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
+++ b/Tracking_sheet/Tech_Savy_Timesheet_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My_Project\CMPE-243\cmpe243_techsavy_rc_car\Tracking_sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KIRIT MAKANI\cmpe243_techsavy_rc_car\Tracking_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B97D116-4784-4603-8E93-771AF4E00037}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B22BF23-31C5-4DDB-963F-D9625565CA84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defines" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -180,7 +180,73 @@
 3. Displayed the discovered bluetooth devices in a list view</t>
   </si>
   <si>
-    <t>Bridge</t>
+    <t>1. Pushed Bridge code to gitlab
+2. Hardware Interfaced compass with Sjone Board (5v)</t>
+  </si>
+  <si>
+    <t>Documentation &amp; Interfacing</t>
+  </si>
+  <si>
+    <t>BRIDGE &amp; 
+GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go through CMPS 11 datasheet in i2c &amp; Serial Mode and read about it register settings and configurations </t>
+  </si>
+  <si>
+    <t>CMPS 11 - GEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Sheet Reviewing </t>
+  </si>
+  <si>
+    <t>1. Updated wiki report with Project Title details and Car Top &amp; side views.
+2. Added Abstract and How self driving car works on Wiki.
+3. Added Introduction &amp; onjectives of Tech Savy on Wiki with High Level System Design.</t>
+  </si>
+  <si>
+    <t>1. Updated wiki report with  Team Members &amp; Technical Responsibilities.
+2. Updated wiki report with  Team Members &amp;   Administrative Responsibilities.
+3. Updated wiki report with  Team Deliverables Schedule.
+4. Added BILL OF MATERIALS (GENERAL PARTS) and Details on the Wiki.
+5. Changed the Wiki Font , format and design for our team and added color codes for all modules.</t>
+  </si>
+  <si>
+    <t>GEO - CMPS11</t>
+  </si>
+  <si>
+    <t>1. Interfacing of CMPS11 with SJONE board on 3.3V.
+2. Interfaced &amp; Implement I2C Mode with CMP11 on SJOne. 
+3. Worked on all axis Calibration of CMPS11 using registers 0xF0, 0xF5 and 0xF6.
+4. Implemented start &amp; stop caliberation mode for CMPS 11 using command registers on SWITCH.
+5. Implemented factory caliberation mode for CMPS11 on Switch in order to revert caliberation.</t>
+  </si>
+  <si>
+    <t>1. Study &amp; Implemented I2C Read/Write functions for CMPS11.
+2. Implemented Heading Angle Calculation Functionality for CMPS11.
+3. Refactoring of code for Geo Controller.
+4. Implemented C wrapper for I2C2.cpp.</t>
+  </si>
+  <si>
+    <t>1. Updated wiki report with  Team Deliverables Schedule Till Final Demo
+2. Updated HW Block Diagrams for Bluetooth and Geo Controller</t>
+  </si>
+  <si>
+    <t>Hardware Design and Motor Control</t>
+  </si>
+  <si>
+    <t>4,5,6</t>
+  </si>
+  <si>
+    <t>PCB and Motor Controller</t>
+  </si>
+  <si>
+    <t>1. Tested RC car DC and Servo Motor with the basic PWM API driver and performed ESC calibration before starting the motor
+2. Started designing schematics and PCB layout for the RC car project      3. Designed power circuit and identified the components required(BOM)   4. Updated changes to schematic based on the previous project and team's inputs
+5. Helped Jay to develop motor driver implementing CAN and DBC</t>
+  </si>
+  <si>
+    <t>20 (Combined for week 4,5,6)</t>
   </si>
 </sst>
 </file>
@@ -263,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,7 +359,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,14 +679,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.69921875" customWidth="1"/>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -643,7 +708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -654,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -665,7 +730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -676,7 +741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -687,7 +752,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -698,7 +763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -709,7 +774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -717,17 +782,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -739,25 +804,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -780,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43553</v>
       </c>
@@ -803,7 +868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43553</v>
       </c>
@@ -826,11 +891,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43553</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="8">
+        <v>5</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>42</v>
       </c>
@@ -847,11 +914,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43554</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8">
+        <v>5</v>
+      </c>
       <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
@@ -868,11 +937,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43555</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
       <c r="C6" s="8" t="s">
         <v>43</v>
       </c>
@@ -889,24 +960,211 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>43555</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="E7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>43556</v>
+      </c>
+      <c r="B8" s="8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>43557</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>43558</v>
+      </c>
+      <c r="B10" s="8">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>43559</v>
+      </c>
+      <c r="B11" s="8">
+        <v>5</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="8">
+        <v>4</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="102" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>43560</v>
+      </c>
+      <c r="B12" s="8">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="8">
+        <v>4</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>43561</v>
+      </c>
+      <c r="B13" s="8">
+        <v>5</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="8">
+        <v>4</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>43563</v>
+      </c>
+      <c r="B14" s="8">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="8">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>43565</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>